<commit_message>
Read specific colunm .xlsx with Python
</commit_message>
<xml_diff>
--- a/pessoas.xlsx
+++ b/pessoas.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Nome</t>
   </si>
@@ -67,14 +67,37 @@
   </si>
   <si>
     <t>1.86</t>
+  </si>
+  <si>
+    <t>Dado1</t>
+  </si>
+  <si>
+    <t>Dado2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Leitura coluna "k"</t>
+  </si>
+  <si>
+    <t>Leitura coluna "l"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -90,7 +113,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -98,12 +121,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,101 +444,135 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="11" max="11" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.1796875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
+    <row r="1" spans="1:12">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="K1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
+    <row r="2" spans="1:12">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>23</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="J2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
+    <row r="3" spans="1:12">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>24</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
+    <row r="4" spans="1:12">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>22</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
+    <row r="5" spans="1:12">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>23</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
+    <row r="6" spans="1:12">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>23</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="J8" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="K2:K6"/>
+    <mergeCell ref="L2:L6"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Testes de leitura e ordenação de dados
</commit_message>
<xml_diff>
--- a/pessoas.xlsx
+++ b/pessoas.xlsx
@@ -16,19 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
-  <si>
-    <t>Nome</t>
-  </si>
-  <si>
-    <t>Idade</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estado </t>
-  </si>
-  <si>
-    <t>Altura</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>Lucas</t>
   </si>
@@ -69,35 +57,24 @@
     <t>1.86</t>
   </si>
   <si>
-    <t>Dado1</t>
-  </si>
-  <si>
-    <t>Dado2</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Leitura coluna "k"</t>
-  </si>
-  <si>
-    <t>Leitura coluna "l"</t>
+    <t>nome</t>
+  </si>
+  <si>
+    <t>idade</t>
+  </si>
+  <si>
+    <t>estado</t>
+  </si>
+  <si>
+    <t>altura</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -140,16 +117,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -456,121 +427,91 @@
     <col min="12" max="12" width="15.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="B2" s="1">
         <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1">
         <v>24</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
+        <v>9</v>
+      </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1">
         <v>22</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
+        <v>10</v>
+      </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1">
         <v>23</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
+        <v>11</v>
+      </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1">
         <v>23</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="J8" s="3"/>
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="K2:K6"/>
-    <mergeCell ref="L2:L6"/>
-  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>